<commit_message>
Initial voice agent commit 🎙️✨
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -835,6 +835,25 @@
         <v>8.465195417404175</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>session_001</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>7.328892469406128</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2.722530126571655</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.859208822250366</v>
+      </c>
+      <c r="E21" t="n">
+        <v>11.91063141822815</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>